<commit_message>
editing NN and adding Class diagram
</commit_message>
<xml_diff>
--- a/Docs/Tables/NN Attributes.xlsx
+++ b/Docs/Tables/NN Attributes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdelrahman Bonna\Documents\GitHub\Healthy_Shield_Analysis\Docs\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87896BEA-A256-4377-9F7D-195918AB4987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1584191F-AF10-4EC6-99DB-0142B870A79D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Age</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Percentage</t>
   </si>
   <si>
-    <t>60&lt;n</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
@@ -76,6 +73,27 @@
   </si>
   <si>
     <t>single</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>&lt;800</t>
+  </si>
+  <si>
+    <t>2013&lt;model</t>
+  </si>
+  <si>
+    <t>&gt;800</t>
+  </si>
+  <si>
+    <t>2013&gt;model</t>
+  </si>
+  <si>
+    <t>60&lt;=n</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -443,7 +461,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,22 +523,82 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5">
+        <v>3000</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="M2" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3000</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
       <c r="M3" s="6">
         <v>1</v>
       </c>
@@ -576,16 +654,25 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J14" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="M14" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="M15" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" s="5">
+        <v>3</v>
+      </c>
       <c r="M16" s="6">
         <v>0</v>
       </c>

</xml_diff>